<commit_message>
Docs to simulate output and methods
</commit_message>
<xml_diff>
--- a/Docs/DemoData.xlsx
+++ b/Docs/DemoData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current Condition" sheetId="1" r:id="rId1"/>
     <sheet name="Potential Uplift" sheetId="3" r:id="rId2"/>
+    <sheet name="Wtd Overlay" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -20,7 +21,41 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These are predictions from the GLM/RF/MaxEnt models for each catchment.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>NHD Catchment</t>
   </si>
@@ -88,6 +123,57 @@
   </si>
   <si>
     <t>Percentile</t>
+  </si>
+  <si>
+    <t>Delta 1</t>
+  </si>
+  <si>
+    <t>Delta 2</t>
+  </si>
+  <si>
+    <t>Delta 3</t>
+  </si>
+  <si>
+    <t>Delta 4</t>
+  </si>
+  <si>
+    <t>Delta 5</t>
+  </si>
+  <si>
+    <t>Delta 6</t>
+  </si>
+  <si>
+    <t>Delta 7</t>
+  </si>
+  <si>
+    <t>Delta 8</t>
+  </si>
+  <si>
+    <t>Mean Delta</t>
+  </si>
+  <si>
+    <t>Uplift Index</t>
+  </si>
+  <si>
+    <t>Habitat Uplift</t>
+  </si>
+  <si>
+    <t>Geomorph Uplift</t>
+  </si>
+  <si>
+    <t>Hydrology Uplift</t>
+  </si>
+  <si>
+    <t>Water Qual Uplift</t>
+  </si>
+  <si>
+    <t>HUC 12</t>
+  </si>
+  <si>
+    <t>Wt</t>
+  </si>
+  <si>
+    <t>Wtd Uplift</t>
   </si>
 </sst>
 </file>
@@ -97,7 +183,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +226,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +266,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -184,11 +302,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +354,82 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -527,870 +736,928 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="8" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="8" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>30186</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>0.74</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0.99</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>0.01</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>0.22</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.12</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>0.54</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0.91</v>
       </c>
-      <c r="J2" s="3">
-        <f>AVERAGE(B2:I2)</f>
+      <c r="K2" s="3">
+        <f>AVERAGE(C2:J2)</f>
         <v>0.45</v>
       </c>
-      <c r="K2" s="11">
-        <f>_xlfn.RANK.AVG(J2,J:J,1)</f>
+      <c r="L2" s="11">
+        <f>_xlfn.RANK.AVG(K2,K:K,1)</f>
         <v>8</v>
       </c>
-      <c r="L2" s="11">
-        <f>K2/MAX(K:K)</f>
+      <c r="M2" s="11">
+        <f>L2/MAX(L:L)</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="M2" s="9" t="str">
-        <f>IF(L2&gt;0.8,"Good",IF(L2&gt;0.2,"Restorable","Beyond repair"))</f>
+      <c r="N2" s="9" t="str">
+        <f>IF(M2&gt;0.8,"Good",IF(M2&gt;0.2,"Restorable","Beyond repair"))</f>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>30187</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>0.65</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.39</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>0.72</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>0.36</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0.87</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>0.3</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0.94</v>
       </c>
-      <c r="J3" s="3">
-        <f t="shared" ref="J3:J19" si="0">AVERAGE(B3:I3)</f>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K19" si="0">AVERAGE(C3:J3)</f>
         <v>0.59124999999999994</v>
       </c>
-      <c r="K3" s="11">
-        <f t="shared" ref="K3:K19" si="1">_xlfn.RANK.AVG(J3,J:J,1)</f>
+      <c r="L3" s="11">
+        <f t="shared" ref="L3:L19" si="1">_xlfn.RANK.AVG(K3,K:K,1)</f>
         <v>17</v>
       </c>
-      <c r="L3" s="11">
-        <f t="shared" ref="L3:L19" si="2">K3/MAX(K:K)</f>
+      <c r="M3" s="11">
+        <f t="shared" ref="M3:M19" si="2">L3/MAX(L:L)</f>
         <v>0.94444444444444442</v>
       </c>
-      <c r="M3" s="9" t="str">
-        <f t="shared" ref="M3:M19" si="3">IF(L3&gt;0.8,"Good",IF(L3&gt;0.2,"Restorable","Beyond repair"))</f>
+      <c r="N3" s="9" t="str">
+        <f t="shared" ref="N3:N19" si="3">IF(M3&gt;0.8,"Good",IF(M3&gt;0.2,"Restorable","Beyond repair"))</f>
         <v>Good</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
         <v>30188</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>0.96</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.25</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.78</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.22</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.42</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>0.44</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>0.48</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.32</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <f t="shared" si="0"/>
         <v>0.48374999999999996</v>
       </c>
-      <c r="K4" s="11">
+      <c r="L4" s="11">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="L4" s="11">
+      <c r="M4" s="11">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="M4" s="9" t="str">
+      <c r="N4" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>30189</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>0.33</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>0.01</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>0.09</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>0.72</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.41</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>0.49</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>0.79</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
         <v>0.42749999999999999</v>
       </c>
-      <c r="K5" s="11">
+      <c r="L5" s="11">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M5" s="9" t="str">
+      <c r="N5" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
         <v>30190</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>0.6</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>0.52</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>0.7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>0.21</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.37</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.69</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>0.01</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.03</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <f t="shared" si="0"/>
         <v>0.39124999999999999</v>
       </c>
-      <c r="K6" s="11">
+      <c r="L6" s="11">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L6" s="11">
+      <c r="M6" s="11">
         <f t="shared" si="2"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="M6" s="9" t="str">
+      <c r="N6" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Beyond repair</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
         <v>30191</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="2">
         <v>0.21</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>0.26</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>0.2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>0.71</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>0.49</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>0.89</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>0.16</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>0.435</v>
       </c>
-      <c r="K7" s="11">
+      <c r="L7" s="11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <f t="shared" si="2"/>
         <v>0.3888888888888889</v>
       </c>
-      <c r="M7" s="9" t="str">
+      <c r="N7" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
         <v>30192</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>0.04</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>0.41</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>0.48</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>0.52</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>0.45</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>0.64</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>0.2</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
         <v>0.41250000000000003</v>
       </c>
-      <c r="K8" s="11">
+      <c r="L8" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="L8" s="11">
+      <c r="M8" s="11">
         <f t="shared" si="2"/>
         <v>0.27777777777777779</v>
       </c>
-      <c r="M8" s="9" t="str">
+      <c r="N8" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
         <v>30193</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>0.44</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>0.11</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>0.39</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0.1</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>0.91</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>0.62</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <f t="shared" si="0"/>
         <v>0.40875000000000006</v>
       </c>
-      <c r="K9" s="11">
+      <c r="L9" s="11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L9" s="11">
+      <c r="M9" s="11">
         <f t="shared" si="2"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="M9" s="9" t="str">
+      <c r="N9" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
         <v>30194</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.61</v>
       </c>
       <c r="C10" s="2">
         <v>0.61</v>
       </c>
       <c r="D10" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="E10" s="2">
         <v>0.91</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0.54</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>0.85</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>0.2</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>0.35</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <f t="shared" si="0"/>
         <v>0.54374999999999996</v>
       </c>
-      <c r="K10" s="11">
+      <c r="L10" s="11">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="L10" s="11">
+      <c r="M10" s="11">
         <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="M10" s="9" t="str">
+      <c r="N10" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="17">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
         <v>30195</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C11" s="2">
         <v>0.5</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>0.91</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>0.64</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>0.26</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.47</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>0.95</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>0.8</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
         <v>0.57500000000000007</v>
       </c>
-      <c r="K11" s="11">
+      <c r="L11" s="11">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="L11" s="11">
+      <c r="M11" s="11">
         <f t="shared" si="2"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="M11" s="9" t="str">
+      <c r="N11" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Good</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="17">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
         <v>30196</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C12" s="2">
         <v>0.78</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>0.37</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>0.18</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>0.72</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>0.67</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>0.7</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>0.97</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <f t="shared" si="0"/>
         <v>0.61874999999999991</v>
       </c>
-      <c r="K12" s="11">
+      <c r="L12" s="11">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="L12" s="11">
+      <c r="M12" s="11">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M12" s="9" t="str">
+      <c r="N12" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Good</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="17">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
         <v>30197</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C13" s="2">
         <v>0.68</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>0.98</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>0.15</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>0.83</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>0.5</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>0.3</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>0.64</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>0.31</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
         <v>0.54874999999999996</v>
       </c>
-      <c r="K13" s="11">
+      <c r="L13" s="11">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="L13" s="11">
+      <c r="M13" s="11">
         <f t="shared" si="2"/>
         <v>0.72222222222222221</v>
       </c>
-      <c r="M13" s="9" t="str">
+      <c r="N13" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="17">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
         <v>30198</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C14" s="2">
         <v>0.84</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.39</v>
       </c>
       <c r="D14" s="2">
         <v>0.39</v>
       </c>
       <c r="E14" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="F14" s="2">
         <v>0.42</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.76</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>0.19</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>0.82</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>0.76</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <f t="shared" si="0"/>
         <v>0.57124999999999992</v>
       </c>
-      <c r="K14" s="11">
+      <c r="L14" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="L14" s="11">
+      <c r="M14" s="11">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M14" s="9" t="str">
+      <c r="N14" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Good</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="17">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
         <v>30199</v>
       </c>
-      <c r="B15" s="2">
+      <c r="C15" s="2">
         <v>0.72</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>0.24</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>0.25</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>0.54</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>0.36</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>0.31</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>0.06</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>0.43</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
         <v>0.36375000000000002</v>
       </c>
-      <c r="K15" s="11">
+      <c r="L15" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L15" s="11">
+      <c r="M15" s="11">
         <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="M15" s="9" t="str">
+      <c r="N15" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Beyond repair</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="17">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
         <v>30200</v>
       </c>
-      <c r="B16" s="2">
+      <c r="C16" s="2">
         <v>0.67</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>0.01</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>0.91</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>0.71</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>0.01</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>0.17</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>0.99</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
         <v>0.50249999999999995</v>
       </c>
-      <c r="K16" s="11">
+      <c r="L16" s="11">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="L16" s="11">
+      <c r="M16" s="11">
         <f t="shared" si="2"/>
         <v>0.55555555555555558</v>
       </c>
-      <c r="M16" s="9" t="str">
+      <c r="N16" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1">
         <v>30201</v>
       </c>
-      <c r="B17" s="2">
+      <c r="C17" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C17" s="2">
+      <c r="D17" s="2">
         <v>0.13</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>0.74</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>0.03</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.24</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>0.4</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>0.06</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>0.3</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <f t="shared" si="0"/>
         <v>0.255</v>
       </c>
-      <c r="K17" s="11">
+      <c r="L17" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L17" s="11">
+      <c r="M17" s="11">
         <f t="shared" si="2"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="M17" s="9" t="str">
+      <c r="N17" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Beyond repair</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
         <v>30202</v>
       </c>
-      <c r="B18" s="2">
+      <c r="C18" s="2">
         <v>0.74</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>0.43</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>0.08</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>0.11</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0.76</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>0.69</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>0.66</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>0.98</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <f t="shared" si="0"/>
         <v>0.55625000000000002</v>
       </c>
-      <c r="K18" s="11">
+      <c r="L18" s="11">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="L18" s="11">
+      <c r="M18" s="11">
         <f t="shared" si="2"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="M18" s="9" t="str">
+      <c r="N18" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
         <v>30203</v>
       </c>
-      <c r="B19" s="2">
+      <c r="C19" s="2">
         <v>0.35</v>
       </c>
-      <c r="C19" s="2">
+      <c r="D19" s="2">
         <v>0.77</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>0.26</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>0.82</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>0.9</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>0.42</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>0.53</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <f t="shared" si="0"/>
         <v>0.50624999999999998</v>
       </c>
-      <c r="K19" s="11">
+      <c r="L19" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="L19" s="11">
+      <c r="M19" s="11">
         <f t="shared" si="2"/>
         <v>0.61111111111111116</v>
       </c>
-      <c r="M19" s="9" t="str">
+      <c r="N19" s="9" t="str">
         <f t="shared" si="3"/>
         <v>Restorable</v>
       </c>
@@ -1399,22 +1666,1044 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J2 J3:J19" formulaRange="1"/>
+    <ignoredError sqref="K2 K3:K19" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="M2" sqref="M2:M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="12" width="9.140625" style="16"/>
+    <col min="13" max="13" width="10" style="22" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17">
+        <v>30186</v>
+      </c>
+      <c r="C2" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="D2" s="18">
+        <v>0.48</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.31</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="H2" s="18">
+        <v>0.21</v>
+      </c>
+      <c r="I2" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K2" s="19">
+        <f>AVERAGE(C2:J2)</f>
+        <v>0.38</v>
+      </c>
+      <c r="L2" s="20">
+        <f>_xlfn.RANK.AVG(K2,K:K,1)</f>
+        <v>18</v>
+      </c>
+      <c r="M2" s="21">
+        <f>L2/MAX(L:L)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="17">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <v>30187</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F3" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="K3" s="19">
+        <f t="shared" ref="K3:K19" si="0">AVERAGE(C3:J3)</f>
+        <v>0.2</v>
+      </c>
+      <c r="L3" s="20">
+        <f t="shared" ref="L3:L19" si="1">_xlfn.RANK.AVG(K3,K:K,1)</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="21">
+        <f t="shared" ref="M3:M19" si="2">L3/MAX(L:L)</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="17">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17">
+        <v>30188</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.34</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="H4" s="18">
+        <v>-0.01</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="K4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.16249999999999998</v>
+      </c>
+      <c r="L4" s="20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M4" s="21">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="17">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17">
+        <v>30189</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="D5" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="E5" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F5" s="18">
+        <v>0.43</v>
+      </c>
+      <c r="G5" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="I5" s="18">
+        <v>0.36</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="K5" s="19">
+        <f t="shared" si="0"/>
+        <v>0.3175</v>
+      </c>
+      <c r="L5" s="20">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="M5" s="21">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="17">
+        <v>2</v>
+      </c>
+      <c r="B6" s="17">
+        <v>30190</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.48</v>
+      </c>
+      <c r="G6" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="18">
+        <v>0.32</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="K6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="L6" s="20">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="M6" s="21">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="17">
+        <v>2</v>
+      </c>
+      <c r="B7" s="17">
+        <v>30191</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.41</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I7" s="18">
+        <v>0.33</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="L7" s="20">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="M7" s="21">
+        <f t="shared" si="2"/>
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>2</v>
+      </c>
+      <c r="B8" s="17">
+        <v>30192</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.09</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.31</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.06</v>
+      </c>
+      <c r="H8" s="18">
+        <v>0.33</v>
+      </c>
+      <c r="I8" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="J8" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="K8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.18625</v>
+      </c>
+      <c r="L8" s="20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="M8" s="21">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="17">
+        <v>3</v>
+      </c>
+      <c r="B9" s="17">
+        <v>30193</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="G9" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="I9" s="18">
+        <v>0.33</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="K9" s="19">
+        <f t="shared" si="0"/>
+        <v>0.2525</v>
+      </c>
+      <c r="L9" s="20">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M9" s="21">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17">
+        <v>30194</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.23</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0.21</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.46</v>
+      </c>
+      <c r="K10" s="19">
+        <f t="shared" si="0"/>
+        <v>0.32624999999999998</v>
+      </c>
+      <c r="L10" s="20">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="M10" s="21">
+        <f t="shared" si="2"/>
+        <v>0.94444444444444442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="17">
+        <v>3</v>
+      </c>
+      <c r="B11" s="17">
+        <v>30195</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.39</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.48</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="G11" s="18">
+        <v>0.05</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I11" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K11" s="19">
+        <f t="shared" si="0"/>
+        <v>0.23375000000000004</v>
+      </c>
+      <c r="L11" s="20">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M11" s="21">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="17">
+        <v>3</v>
+      </c>
+      <c r="B12" s="17">
+        <v>30196</v>
+      </c>
+      <c r="C12" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.23</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.38</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="K12" s="19">
+        <f t="shared" si="0"/>
+        <v>0.29374999999999996</v>
+      </c>
+      <c r="L12" s="20">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="M12" s="21">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="17">
+        <v>4</v>
+      </c>
+      <c r="B13" s="17">
+        <v>30197</v>
+      </c>
+      <c r="C13" s="18">
+        <v>0.42</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="F13" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.35</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="J13" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="K13" s="19">
+        <f t="shared" si="0"/>
+        <v>0.24875</v>
+      </c>
+      <c r="L13" s="20">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M13" s="21">
+        <f t="shared" si="2"/>
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="17">
+        <v>4</v>
+      </c>
+      <c r="B14" s="17">
+        <v>30198</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.09</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="F14" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="J14" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="K14" s="19">
+        <f t="shared" si="0"/>
+        <v>0.21625</v>
+      </c>
+      <c r="L14" s="20">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M14" s="21">
+        <f t="shared" si="2"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="17">
+        <v>4</v>
+      </c>
+      <c r="B15" s="17">
+        <v>30199</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="E15" s="18">
+        <v>-0.02</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0.23</v>
+      </c>
+      <c r="J15" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="K15" s="19">
+        <f t="shared" si="0"/>
+        <v>0.20749999999999999</v>
+      </c>
+      <c r="L15" s="20">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="M15" s="21">
+        <f t="shared" si="2"/>
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="17">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17">
+        <v>30200</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.41</v>
+      </c>
+      <c r="F16" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="G16" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="H16" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.19</v>
+      </c>
+      <c r="J16" s="18">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="19">
+        <f t="shared" si="0"/>
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="L16" s="20">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M16" s="21">
+        <f t="shared" si="2"/>
+        <v>0.3888888888888889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17">
+        <v>30201</v>
+      </c>
+      <c r="C17" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0.31</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.48</v>
+      </c>
+      <c r="F17" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.45</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.4</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="J17" s="18">
+        <v>0</v>
+      </c>
+      <c r="K17" s="19">
+        <f t="shared" si="0"/>
+        <v>0.24374999999999999</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="M17" s="21">
+        <f t="shared" si="2"/>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
+        <v>5</v>
+      </c>
+      <c r="B18" s="17">
+        <v>30202</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.16</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="I18" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="J18" s="18">
+        <v>0.17</v>
+      </c>
+      <c r="K18" s="19">
+        <f t="shared" si="0"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="M18" s="21">
+        <f t="shared" si="2"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
+        <v>5</v>
+      </c>
+      <c r="B19" s="17">
+        <v>30203</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0.18</v>
+      </c>
+      <c r="D19" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.16</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0.02</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="I19" s="18">
+        <v>-0.01</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="K19" s="19">
+        <f t="shared" si="0"/>
+        <v>0.11750000000000001</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M19" s="21">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="6" width="11.5703125" style="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="23" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="26">
+        <f>AVERAGEIF('Potential Uplift'!A$2:A$19,A2,'Potential Uplift'!M$2:M$19)</f>
+        <v>0.44444444444444448</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.34</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0.32</v>
+      </c>
+      <c r="E2" s="35">
+        <v>0.78</v>
+      </c>
+      <c r="G2" s="25">
+        <f>B2*B$8+C2*C$8+D2*D$8+E2*E$8</f>
+        <v>0.40511111111111114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26">
+        <f>AVERAGEIF('Potential Uplift'!A$2:A$19,A3,'Potential Uplift'!M$2:M$19)</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.21</v>
+      </c>
+      <c r="D3" s="32">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E3" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="G3" s="25">
+        <f t="shared" ref="G3:G6" si="0">B3*B$8+C3*C$8+D3*D$8+E3*E$8</f>
+        <v>0.39741666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26">
+        <f>AVERAGEIF('Potential Uplift'!A$2:A$19,A4,'Potential Uplift'!M$2:M$19)</f>
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.71</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E4" s="35">
+        <v>0.69</v>
+      </c>
+      <c r="G4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.67702777777777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26">
+        <f>AVERAGEIF('Potential Uplift'!A$2:A$19,A5,'Potential Uplift'!M$2:M$19)</f>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.67</v>
+      </c>
+      <c r="D5" s="32">
+        <v>0.54</v>
+      </c>
+      <c r="E5" s="35">
+        <v>0.26</v>
+      </c>
+      <c r="G5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.53663888888888889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26">
+        <f>AVERAGEIF('Potential Uplift'!A$2:A$19,A6,'Potential Uplift'!M$2:M$19)</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.24</v>
+      </c>
+      <c r="D6" s="32">
+        <v>0.47</v>
+      </c>
+      <c r="E6" s="35">
+        <v>0.46</v>
+      </c>
+      <c r="G6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.37061111111111106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="27">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUM(B8:E8)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>